<commit_message>
Updated Ref. Model and Verf Plan
</commit_message>
<xml_diff>
--- a/ALU_Verf_Plan.xlsx
+++ b/ALU_Verf_Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Graduation Project\Siemens\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Graduation Project\Siemens\ALU_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A86404-397D-4A73-81B8-760D99409F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE473088-455A-4A6B-9F0C-B650B6EA8DCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>Label</t>
   </si>
@@ -167,6 +168,33 @@
   </si>
   <si>
     <t>Covered the SEL, INC, DEC, AND, OR, XOR, SHIFT_L, SHIFT_R, ROTATE_L and ROTATE_R values for the opcode.</t>
+  </si>
+  <si>
+    <t>ALU_8</t>
+  </si>
+  <si>
+    <t>ALU_9</t>
+  </si>
+  <si>
+    <t>When Valid_in = 1, input is valid, so output values adjust and valid_out = 1.</t>
+  </si>
+  <si>
+    <t>Covering invalid inputs and outputs.</t>
+  </si>
+  <si>
+    <t>Covering valid inputs and outputs.</t>
+  </si>
+  <si>
+    <t>When Valid_in = 0, input is not valid, so output values don’t change and valid_out = 0.</t>
+  </si>
+  <si>
+    <t>ALU_10</t>
+  </si>
+  <si>
+    <t>Whrn OPCODE = 14 or 15. output stays the same and valid_out = 0.</t>
+  </si>
+  <si>
+    <t>Covering ctl values that aren't of the opcodes.</t>
   </si>
 </sst>
 </file>
@@ -556,9 +584,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E965"/>
+  <dimension ref="A1:E968"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="56" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -674,7 +702,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>27</v>
       </c>
@@ -708,128 +736,158 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>8</v>
+    <row r="9" spans="1:5" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>10</v>
+        <v>52</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>11</v>
+        <v>53</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
+      <c r="D13" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="53.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
+      <c r="D14" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+    <row r="15" spans="1:5" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -7467,6 +7525,27 @@
       <c r="D965" s="6"/>
       <c r="E965" s="6"/>
     </row>
+    <row r="966" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A966" s="9"/>
+      <c r="B966" s="6"/>
+      <c r="C966" s="6"/>
+      <c r="D966" s="6"/>
+      <c r="E966" s="6"/>
+    </row>
+    <row r="967" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A967" s="9"/>
+      <c r="B967" s="6"/>
+      <c r="C967" s="6"/>
+      <c r="D967" s="6"/>
+      <c r="E967" s="6"/>
+    </row>
+    <row r="968" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A968" s="9"/>
+      <c r="B968" s="6"/>
+      <c r="C968" s="6"/>
+      <c r="D968" s="6"/>
+      <c r="E968" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>